<commit_message>
Test case updated for USER STORY #OMS-183 and OMS-488
Test case updated for USER STORY #OMS-183 and OMS-488
</commit_message>
<xml_diff>
--- a/TestData/Bulk_order_Testdata.xlsx
+++ b/TestData/Bulk_order_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ustiws02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779DF951-028B-421B-BF80-E6EE753F3DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC999C4B-CA5A-40D6-8C00-22035ABAAA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
   <si>
     <t>Qty</t>
   </si>
@@ -88,13 +88,82 @@
   </si>
   <si>
     <t>Ingram_SKU</t>
+  </si>
+  <si>
+    <t>MA70</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>JA 0911</t>
+  </si>
+  <si>
+    <t>Header Comment 2</t>
+  </si>
+  <si>
+    <t>Header 2</t>
+  </si>
+  <si>
+    <t>4353CD</t>
+  </si>
+  <si>
+    <t>4353CC</t>
+  </si>
+  <si>
+    <t>4353DD</t>
+  </si>
+  <si>
+    <t>43ABCD</t>
+  </si>
+  <si>
+    <t>AB53CD</t>
+  </si>
+  <si>
+    <t>Header Comment 3</t>
+  </si>
+  <si>
+    <t>Header Comment 4</t>
+  </si>
+  <si>
+    <t>Header Comment 5</t>
+  </si>
+  <si>
+    <t>Header Comment 6</t>
+  </si>
+  <si>
+    <t>Header Comment 7</t>
+  </si>
+  <si>
+    <t>Header Comment 8</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Header 3</t>
+  </si>
+  <si>
+    <t>Header 4</t>
+  </si>
+  <si>
+    <t>Header 5</t>
+  </si>
+  <si>
+    <t>Header 6</t>
+  </si>
+  <si>
+    <t>Header 7</t>
+  </si>
+  <si>
+    <t>Header 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,16 +199,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -162,11 +254,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -174,6 +307,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,7 +750,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -649,7 +788,274 @@
         <v>124</v>
       </c>
     </row>
+    <row r="6" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="8">
+        <v>435363</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[OMS-2851] Updated code for bug fixing
</commit_message>
<xml_diff>
--- a/TestData/Bulk_order_Testdata.xlsx
+++ b/TestData/Bulk_order_Testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ustiws02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC999C4B-CA5A-40D6-8C00-22035ABAAA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907345F8-BC69-40B8-9384-2049FF7ABAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>Qty</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Header 8</t>
+  </si>
+  <si>
+    <t>Header Comment 1</t>
+  </si>
+  <si>
+    <t>Header 1</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +727,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -757,35 +763,35 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2022222</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5">
         <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5">
-        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
test update for OMS-777, OMS-3046, OMS-3470
Automation test case written for OMS-777, OMS-3046, OMS-3470
</commit_message>
<xml_diff>
--- a/TestData/Bulk_order_Testdata.xlsx
+++ b/TestData/Bulk_order_Testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ustiws02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907345F8-BC69-40B8-9384-2049FF7ABAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1932494-8C81-4070-9CF6-DE6701E5DEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="64">
   <si>
     <t>Qty</t>
   </si>
@@ -163,6 +163,60 @@
   </si>
   <si>
     <t>Header 1</t>
+  </si>
+  <si>
+    <t>Vendor_Part_Number</t>
+  </si>
+  <si>
+    <t>E025SLL-H</t>
+  </si>
+  <si>
+    <t>46694G</t>
+  </si>
+  <si>
+    <t>19853H</t>
+  </si>
+  <si>
+    <t>Two_Null_Value</t>
+  </si>
+  <si>
+    <t>One_Null_Value</t>
+  </si>
+  <si>
+    <t>Three_Null_Value</t>
+  </si>
+  <si>
+    <t>Sku_And_Vendor_Part_No</t>
+  </si>
+  <si>
+    <t>Null_Sku_and_Vendor_Part_No</t>
+  </si>
+  <si>
+    <t>Sku_And_Vendor_Part_No_Mismatch</t>
+  </si>
+  <si>
+    <t>Header Comment 9</t>
+  </si>
+  <si>
+    <t>Header Comment 10</t>
+  </si>
+  <si>
+    <t>Header Comment 11</t>
+  </si>
+  <si>
+    <t>Header 9</t>
+  </si>
+  <si>
+    <t>Header 10</t>
+  </si>
+  <si>
+    <t>Header 11</t>
+  </si>
+  <si>
+    <t>Single_Order</t>
+  </si>
+  <si>
+    <t>Multiple_Order</t>
   </si>
 </sst>
 </file>
@@ -599,18 +653,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
@@ -622,7 +677,7 @@
     <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -659,13 +714,16 @@
       <c r="L1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="M1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>51</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -695,12 +753,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -727,12 +785,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -756,12 +814,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>4</v>
+      <c r="B5" t="s">
+        <v>62</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>21</v>
@@ -794,12 +852,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>5</v>
+      <c r="B6" t="s">
+        <v>63</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>21</v>
@@ -832,12 +890,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>5</v>
+      <c r="B7" t="s">
+        <v>63</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>21</v>
@@ -870,12 +928,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>5</v>
+      <c r="B8" t="s">
+        <v>63</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>21</v>
@@ -908,12 +966,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>5</v>
+      <c r="B9" t="s">
+        <v>63</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>21</v>
@@ -946,12 +1004,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>5</v>
+      <c r="B10" t="s">
+        <v>63</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>21</v>
@@ -984,12 +1042,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>5</v>
+      <c r="B11" t="s">
+        <v>63</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>21</v>
@@ -1022,12 +1080,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>5</v>
+      <c r="B12" t="s">
+        <v>63</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>21</v>
@@ -1059,6 +1117,138 @@
       <c r="L12">
         <v>1</v>
       </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="6">
+        <v>10066860</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>